<commit_message>
Changes to exercise 'Overview' sheet
</commit_message>
<xml_diff>
--- a/xlsx/sample-spreadsheet2.xlsx
+++ b/xlsx/sample-spreadsheet2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkrepp.AD\process-bp-count-spreadsheets\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87F0239-1CA2-40DD-91BE-E5922C53F457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4A6A73-5957-41E3-941F-787ADCE96716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23280" yWindow="216" windowWidth="21600" windowHeight="12192" xr2:uid="{0C6062F5-86F8-4814-A110-428A3D225A11}"/>
   </bookViews>
@@ -1625,28 +1625,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1656,6 +1638,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1999,7 +1999,7 @@
   <dimension ref="B1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2020,41 +2020,45 @@
       <c r="B2" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="11" t="s">
+      <c r="C2" s="7">
+        <v>45223</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>443</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="15" t="s">
+      <c r="E2" s="18"/>
+      <c r="F2" s="20" t="s">
         <v>331</v>
       </c>
-      <c r="G2" s="15"/>
+      <c r="G2" s="20"/>
       <c r="H2" s="10"/>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="18" t="s">
         <v>304</v>
       </c>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
     </row>
     <row r="3" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
+      <c r="C3" s="8">
+        <v>65</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
       <c r="H3" s="10"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
     </row>
     <row r="4" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
@@ -2063,187 +2067,171 @@
       <c r="C4" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
       <c r="H4" s="10"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="17" t="s">
+        <v>347</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
       <c r="H5" s="1">
         <f>VLOOKUP(D5,Columns!$D$3:$E$272,2,0)</f>
-        <v>20179</v>
-      </c>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
+        <v>20058</v>
+      </c>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
     </row>
     <row r="6" spans="2:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="12" t="s">
         <v>352</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="17"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
       <c r="H6" s="1"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="11" t="s">
         <v>323</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="21"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="15"/>
       <c r="H7" s="1"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="11" t="s">
         <v>324</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="12" t="s">
+      <c r="C8" s="11"/>
+      <c r="D8" s="17" t="s">
         <v>316</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
       <c r="H8" s="2"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
     </row>
     <row r="9" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="12" t="s">
         <v>442</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
       <c r="H9" s="1"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="11" t="s">
         <v>325</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="12" t="s">
+      <c r="C10" s="11"/>
+      <c r="D10" s="17" t="s">
         <v>316</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
       <c r="H10" s="2"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="12" t="s">
-        <v>425</v>
-      </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="17" t="s">
+        <v>424</v>
+      </c>
+      <c r="E11" s="17"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
       <c r="H11" s="1"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="17"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
       <c r="H12" s="1"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="J2:O3"/>
-    <mergeCell ref="D11:E11"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="F8:G8"/>
@@ -2251,9 +2239,25 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="F12:G12"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="J2:O3"/>
+    <mergeCell ref="D11:E11"/>
     <mergeCell ref="D2:E4"/>
     <mergeCell ref="F2:G4"/>
     <mergeCell ref="J4:O12"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{B33F18CB-4361-4EA4-89CA-2CFFDEBFD17B}">

</xml_diff>